<commit_message>
added post on tippeligaen
</commit_message>
<xml_diff>
--- a/content/data/tippeliga_2019.xlsx
+++ b/content/data/tippeliga_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kauna\Documents\R\test_blogdown\content\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECAF73C-6A3A-459B-A70D-80C9A6DE56B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF89A28-39D1-4B14-BF33-D4DBC63DC64E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F01B593A-E404-461A-8214-9D818D1F28AE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$E$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$H$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>NordicBet</t>
   </si>
@@ -118,16 +118,42 @@
   </si>
   <si>
     <t>https://www.oddschecker.com/football/norway/eliteserien/norwegian-eliteserien/winner</t>
+  </si>
+  <si>
+    <t>Dagsavisen</t>
+  </si>
+  <si>
+    <t>Dagbladet</t>
+  </si>
+  <si>
+    <t>https://www.dagbladet.no/sport/dagbladets-tabelltips-slik-ender-eliteserien/70922152</t>
+  </si>
+  <si>
+    <t>https://www.dagsavisen.no/sport/slik-ender-eliteserien-kanskje-1.1457870</t>
+  </si>
+  <si>
+    <t>Aftenposten</t>
+  </si>
+  <si>
+    <t>https://www.aftenposten.no/100Sport/fotball/Bare-n-av-fem-eksperter-tror-pa-RBK-gull---I-dag-er-de-ikke-i-narheten-av-topp-tre-271547b.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,13 +176,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,15 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE54E0-964A-4484-9C17-EC4F953FB6AA}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -493,208 +522,362 @@
       <c r="E1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="H2">
+        <f>(1+1+1+2+1)/5</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <f>(2+2+2+1+2)/5</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f>(4+3+3+3+3)/5</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <f>(3+4+8+8+8)/5</f>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
       <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="C8">
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
       <c r="D10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>15</v>
+      </c>
+      <c r="G12">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="H12">
+        <f>(15+(8*4))/5</f>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>9</v>
       </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
+      <c r="C13">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="G13">
         <v>15</v>
       </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13">
+      <c r="H13">
+        <f>(15+(8*4))/5</f>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
         <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>14</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
       <c r="E14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <f>(14+14+13+8+8)/5</f>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -710,49 +893,79 @@
       <c r="E15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <f>(15+14+14+8+8)/5</f>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16">
         <v>13</v>
       </c>
-      <c r="C16">
+      <c r="H16">
+        <f>(16+15+15+14+8)/5</f>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
         <v>12</v>
       </c>
-      <c r="D16">
+      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="D17">
         <v>13</v>
       </c>
-      <c r="E16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
+      <c r="E17">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-      <c r="E17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <f>(16+16+16+16+8)/5</f>
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
@@ -761,8 +974,17 @@
       <c r="E19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -771,14 +993,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E17" xr:uid="{252527F8-D078-49F9-8C1E-5FCD8214D8C7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">
-      <sortCondition ref="E1:E17"/>
+  <autoFilter ref="A1:H17" xr:uid="{23C4FACE-132A-4736-AB1A-6F046EDE558B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
+      <sortCondition ref="H1:H17"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
     <sortCondition ref="A2:A17"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1" location="?cat=&amp;reg=&amp;sc=6054" xr:uid="{B7EC5238-1429-4844-9A4C-C1A8354D4A0F}"/>
+    <hyperlink ref="C19" r:id="rId2" xr:uid="{FF0C2C42-C4A2-49D4-AAF2-F0C7BA07787C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>